<commit_message>
KPI for health care industry
</commit_message>
<xml_diff>
--- a/Domains and KPI's.xlsx
+++ b/Domains and KPI's.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20055" windowHeight="7950"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="20055" windowHeight="7950" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="KPI Names" sheetId="1" r:id="rId1"/>
+    <sheet name="Health Care Industry KPIs" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
   <si>
     <t>Domain</t>
   </si>
@@ -142,6 +142,72 @@
   </si>
   <si>
     <t>Threat detection, identity management, compliance tools</t>
+  </si>
+  <si>
+    <t>Occupancy Rate</t>
+  </si>
+  <si>
+    <t>KPI</t>
+  </si>
+  <si>
+    <t>Short Description</t>
+  </si>
+  <si>
+    <t>Bed Occupancy Rate.</t>
+  </si>
+  <si>
+    <t>Average Treatment Cost</t>
+  </si>
+  <si>
+    <t>Average Treatment Cost of patients.</t>
+  </si>
+  <si>
+    <t>Average Patient Wait Time</t>
+  </si>
+  <si>
+    <t>Average Time a patient waits for the appointment.</t>
+  </si>
+  <si>
+    <t>Cancellation Rate</t>
+  </si>
+  <si>
+    <t>After Appointment does patient cancel the appointments.</t>
+  </si>
+  <si>
+    <t>Patients Satisfaction</t>
+  </si>
+  <si>
+    <t>If Patient is satisfied.</t>
+  </si>
+  <si>
+    <t>Average Hospital Stay</t>
+  </si>
+  <si>
+    <t>How much time patient stayed in hospital for treatment.</t>
+  </si>
+  <si>
+    <t>Revisits Rate</t>
+  </si>
+  <si>
+    <t>How often patient comes for treatment.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wait Time </t>
+  </si>
+  <si>
+    <t>Wait time for getting beds.</t>
+  </si>
+  <si>
+    <t>Moratality Rate</t>
+  </si>
+  <si>
+    <t>Number of Emergency Case.</t>
+  </si>
+  <si>
+    <t>MR calculcations.</t>
+  </si>
+  <si>
+    <t>Emergency cases takled by hospital.</t>
   </si>
 </sst>
 </file>
@@ -492,8 +558,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -502,7 +568,7 @@
     <col min="2" max="2" width="54.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="30">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -510,7 +576,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="165">
+    <row r="2" spans="1:2" ht="30">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -518,7 +584,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="135">
+    <row r="3" spans="1:2" ht="30">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -526,7 +592,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="150">
+    <row r="4" spans="1:2" ht="30">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -534,7 +600,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="120">
+    <row r="5" spans="1:2" ht="30">
       <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
@@ -542,7 +608,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="105">
+    <row r="6" spans="1:2">
       <c r="A6" s="3" t="s">
         <v>10</v>
       </c>
@@ -550,7 +616,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="135">
+    <row r="7" spans="1:2" ht="30">
       <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
@@ -558,7 +624,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="120">
+    <row r="8" spans="1:2" ht="30">
       <c r="A8" s="3" t="s">
         <v>14</v>
       </c>
@@ -566,7 +632,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="150">
+    <row r="9" spans="1:2" ht="30">
       <c r="A9" s="3" t="s">
         <v>16</v>
       </c>
@@ -574,7 +640,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="90">
+    <row r="10" spans="1:2">
       <c r="A10" s="3" t="s">
         <v>18</v>
       </c>
@@ -582,7 +648,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="135">
+    <row r="11" spans="1:2" ht="30">
       <c r="A11" s="3" t="s">
         <v>20</v>
       </c>
@@ -590,7 +656,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="135">
+    <row r="12" spans="1:2" ht="30">
       <c r="A12" s="3" t="s">
         <v>22</v>
       </c>
@@ -598,7 +664,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="120">
+    <row r="13" spans="1:2" ht="30">
       <c r="A13" s="3" t="s">
         <v>24</v>
       </c>
@@ -606,7 +672,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="105">
+    <row r="14" spans="1:2" ht="30">
       <c r="A14" s="3" t="s">
         <v>26</v>
       </c>
@@ -614,7 +680,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="90">
+    <row r="15" spans="1:2">
       <c r="A15" s="3" t="s">
         <v>28</v>
       </c>
@@ -622,7 +688,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="105">
+    <row r="16" spans="1:2">
       <c r="A16" s="3" t="s">
         <v>30</v>
       </c>
@@ -630,7 +696,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="135">
+    <row r="17" spans="1:2">
       <c r="A17" s="3" t="s">
         <v>32</v>
       </c>
@@ -638,7 +704,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="90">
+    <row r="18" spans="1:2" ht="30">
       <c r="A18" s="3" t="s">
         <v>34</v>
       </c>
@@ -646,7 +712,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="120">
+    <row r="19" spans="1:2">
       <c r="A19" s="3" t="s">
         <v>36</v>
       </c>
@@ -654,7 +720,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="120">
+    <row r="20" spans="1:2">
       <c r="A20" s="3" t="s">
         <v>38</v>
       </c>
@@ -662,7 +728,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="120">
+    <row r="21" spans="1:2" ht="30">
       <c r="A21" s="3" t="s">
         <v>40</v>
       </c>
@@ -677,12 +743,107 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="30">
+      <c r="A4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B9" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="30">
+      <c r="A11" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B11" t="s">
+        <v>63</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
added more KPIs for health care industry
</commit_message>
<xml_diff>
--- a/Domains and KPI's.xlsx
+++ b/Domains and KPI's.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="76">
   <si>
     <t>Domain</t>
   </si>
@@ -208,6 +208,42 @@
   </si>
   <si>
     <t>Emergency cases takled by hospital.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reference Link </t>
+  </si>
+  <si>
+    <t>https://insightsoftware.com/blog/25-best-healthcare-kpis-and-metric-examples/</t>
+  </si>
+  <si>
+    <t>Staff to Patient Ratio</t>
+  </si>
+  <si>
+    <t>Ratio b/w staff and patients</t>
+  </si>
+  <si>
+    <t>Child Immunization Ratio</t>
+  </si>
+  <si>
+    <t>Child vaccination related KPI</t>
+  </si>
+  <si>
+    <t>Net Profit Margin</t>
+  </si>
+  <si>
+    <t>Net profit margin per year</t>
+  </si>
+  <si>
+    <t>Operating Cashflow</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Current Cashflow Rate.</t>
+  </si>
+  <si>
+    <t>Readmission Rate</t>
+  </si>
+  <si>
+    <t>Readmission of patient to hospital.</t>
   </si>
 </sst>
 </file>
@@ -743,10 +779,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="O16" sqref="O16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -755,23 +791,29 @@
     <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
         <v>43</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="H1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
         <v>42</v>
       </c>
       <c r="B2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="H2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="1" t="s">
         <v>46</v>
       </c>
@@ -779,7 +821,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="30">
+    <row r="4" spans="1:8" ht="30">
       <c r="A4" s="1" t="s">
         <v>48</v>
       </c>
@@ -787,7 +829,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:8">
       <c r="A5" s="1" t="s">
         <v>50</v>
       </c>
@@ -795,7 +837,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:8">
       <c r="A6" s="1" t="s">
         <v>52</v>
       </c>
@@ -803,7 +845,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:8">
       <c r="A7" s="1" t="s">
         <v>54</v>
       </c>
@@ -811,7 +853,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:8">
       <c r="A8" s="1" t="s">
         <v>56</v>
       </c>
@@ -819,7 +861,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:8">
       <c r="A9" s="1" t="s">
         <v>58</v>
       </c>
@@ -827,7 +869,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:8">
       <c r="A10" s="1" t="s">
         <v>60</v>
       </c>
@@ -835,7 +877,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="30">
+    <row r="11" spans="1:8" ht="30">
       <c r="A11" s="1" t="s">
         <v>61</v>
       </c>
@@ -843,8 +885,52 @@
         <v>63</v>
       </c>
     </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B12" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="30">
+      <c r="A13" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B13" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="A14" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B14" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B15" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B16" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Added Automotive sheet in Domain and KPI's
</commit_message>
<xml_diff>
--- a/Domains and KPI's.xlsx
+++ b/Domains and KPI's.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20055" windowHeight="7950" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="20055" windowHeight="7950" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="KPI Names" sheetId="1" r:id="rId1"/>
     <sheet name="Health Care Industry KPIs" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Automotive" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="98">
   <si>
     <t>Domain</t>
   </si>
@@ -244,6 +244,72 @@
   </si>
   <si>
     <t>Readmission of patient to hospital.</t>
+  </si>
+  <si>
+    <t>Monthly Vehicle Sales</t>
+  </si>
+  <si>
+    <t>Number of vehicles sold per month</t>
+  </si>
+  <si>
+    <t>Revenue by Model/Region</t>
+  </si>
+  <si>
+    <t>Revenue broken down by car model or geography</t>
+  </si>
+  <si>
+    <t>Average Selling Price (ASP)</t>
+  </si>
+  <si>
+    <t>Total revenue / number of units sold</t>
+  </si>
+  <si>
+    <t>Dealer Performance</t>
+  </si>
+  <si>
+    <t>Sales performance of dealerships</t>
+  </si>
+  <si>
+    <t>Customer Acquisition Cost (CAC)</t>
+  </si>
+  <si>
+    <t>Cost to acquire one new customer.</t>
+  </si>
+  <si>
+    <t>Formula</t>
+  </si>
+  <si>
+    <t>Total Marketing &amp; Sales Cost / Number of New Customers Acquired</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Total Revenue / Number of Vehicles Sold</t>
+  </si>
+  <si>
+    <t>Inventory Turnover</t>
+  </si>
+  <si>
+    <t>How many times inventory is sold and replaced.</t>
+  </si>
+  <si>
+    <t>Order Fulfillment Time</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Time taken to deliver an order after it’s placed.</t>
+  </si>
+  <si>
+    <t>Warranty Claim Rate</t>
+  </si>
+  <si>
+    <t>(Number of Warranty Claims / Vehicles Sold) * 100</t>
+  </si>
+  <si>
+    <t>Vehicle Defect Rate</t>
+  </si>
+  <si>
+    <t>Number of vehicles returned or repaired due to defects.</t>
+  </si>
+  <si>
+    <t>(Defective Vehicles / Total Vehicles Produced) * 100</t>
   </si>
 </sst>
 </file>
@@ -781,14 +847,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="53.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -936,12 +1002,116 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="35.42578125" customWidth="1"/>
+    <col min="2" max="2" width="52" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="61.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>89</v>
+      </c>
+      <c r="B7" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>91</v>
+      </c>
+      <c r="B8" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>93</v>
+      </c>
+      <c r="B9" t="s">
+        <v>93</v>
+      </c>
+      <c r="C9" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>95</v>
+      </c>
+      <c r="B10" t="s">
+        <v>96</v>
+      </c>
+      <c r="C10" t="s">
+        <v>97</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Sheet for Supply chain and logistics KPI in Domain KPI
</commit_message>
<xml_diff>
--- a/Domains and KPI's.xlsx
+++ b/Domains and KPI's.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20055" windowHeight="7950" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="20055" windowHeight="7950" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="KPI Names" sheetId="1" r:id="rId1"/>
-    <sheet name="Health Care Industry KPIs" sheetId="2" r:id="rId2"/>
+    <sheet name="Health Care Industry" sheetId="2" r:id="rId2"/>
     <sheet name="Automotive" sheetId="3" r:id="rId3"/>
+    <sheet name="Supply Chain Logistics" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="142">
   <si>
     <t>Domain</t>
   </si>
@@ -310,6 +311,138 @@
   </si>
   <si>
     <t>(Defective Vehicles / Total Vehicles Produced) * 100</t>
+  </si>
+  <si>
+    <t>Link=https://www.netsuite.com/portal/resource/articles/inventory-management/logistics-kpis-metrics.shtml</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Order Management</t>
+  </si>
+  <si>
+    <t>Shipping Time</t>
+  </si>
+  <si>
+    <t>Order Accuracy</t>
+  </si>
+  <si>
+    <t>Perfect Order</t>
+  </si>
+  <si>
+    <t>Number of Shipments</t>
+  </si>
+  <si>
+    <t>Supply</t>
+  </si>
+  <si>
+    <t>Lead Time</t>
+  </si>
+  <si>
+    <t>Capacity Utilization</t>
+  </si>
+  <si>
+    <t>Productivity</t>
+  </si>
+  <si>
+    <t>Inventory</t>
+  </si>
+  <si>
+    <t>Customer Backorder Rate</t>
+  </si>
+  <si>
+    <t>Inventory Accuracy</t>
+  </si>
+  <si>
+    <t>Inventory to Sales Ratio</t>
+  </si>
+  <si>
+    <t>Distribution</t>
+  </si>
+  <si>
+    <t>Trailer Utilization Ratio</t>
+  </si>
+  <si>
+    <t>Warehousing Cost</t>
+  </si>
+  <si>
+    <t>Average Dwell Time</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transport Management </t>
+  </si>
+  <si>
+    <t>Delivery Time</t>
+  </si>
+  <si>
+    <t>Average Days Late</t>
+  </si>
+  <si>
+    <t>Freight Payment Accuracy</t>
+  </si>
+  <si>
+    <t>Transporation Cost</t>
+  </si>
+  <si>
+    <t>Shipping time is the length of time it takes for companies to ship an order on or before the requested date. This metric is vital to customer satisfaction. Organizations often couple it with the on-time shipping KPI.</t>
+  </si>
+  <si>
+    <t>Order accuracy is the measure of inventory on-hand and order pick accuracy. </t>
+  </si>
+  <si>
+    <t>KPI that measures how many orders ship without issues (damage, delays or inaccuracies). </t>
+  </si>
+  <si>
+    <t>The number of shipments is how many loads your company sent out in a given period. Looking at the averages of this KPI helps companies optimize their resources and hit their financial goals.</t>
+  </si>
+  <si>
+    <t>also known as order cycle time, is a measure of the time between when a customer places an order and when they receive it</t>
+  </si>
+  <si>
+    <t> Capacity utilization is how much of a resource a company is using.</t>
+  </si>
+  <si>
+    <t>Productivity is a measure of how well a company’s machines, departments and/or people are running.</t>
+  </si>
+  <si>
+    <t>Customer backorder rate is how often a company cannot fulfill an order. This metric directly contributes to customer satisfaction.</t>
+  </si>
+  <si>
+    <t>Inventory accuracy measures how closely your inventory records reflect what is actually in storage. This metric is vital for knowing what your company has in stock and forecasting inventory purchases.</t>
+  </si>
+  <si>
+    <t>also known as stock rotation, is the measure of how many times in a period a company sells all its stock of a certain product.</t>
+  </si>
+  <si>
+    <t>The inventory to sales ratio measures the amount of inventory in stock versus the number of fulfilled sales. </t>
+  </si>
+  <si>
+    <t>Trailer utilization rate measures how well companies are loading their trailers. This rate reflects a company’s load planning and whether it is minimizing costs there as much as possible.</t>
+  </si>
+  <si>
+    <t>Warehousing costs are a group of metrics that cover the expenses specific to your warehouse. These can include any equipment, energy, labor, delivery and shipping costs that get goods into and out of the warehouse. </t>
+  </si>
+  <si>
+    <t>average dwell time, also known as wait time, is the length of time a carrier sits before processing for pickup and delivery. This metric indicates how well a facility functions. Shippers with low average dwell times will struggle to attract drivers and pay more in securing services.</t>
+  </si>
+  <si>
+    <t>also called on-time delivery, measures how quickly an order arrives in full.</t>
+  </si>
+  <si>
+    <t>Average days late is the number of days between the delivery's due date and when the customer receives the order. </t>
+  </si>
+  <si>
+    <t>Truck Turning</t>
+  </si>
+  <si>
+    <t> Truck turning, also known as truck turnaround rate, is the time between when a delivery truck enters a facility to collect or deliver goods and when it exits. The smaller the truck turning rates, the more time the truck is on the road. This rate shows how well a company handles loading and unloading.</t>
+  </si>
+  <si>
+    <t>also called freight bill accuracy, is the number of error-free freight bills compared to the total number of freight bills in a period. </t>
+  </si>
+  <si>
+    <t>Transportation costs are the group of metrics that track an order’s price from beginning to end. This metric includes order processing, administration, inventory carrying costs, warehousing and transportation costs</t>
   </si>
 </sst>
 </file>
@@ -661,7 +794,7 @@
   <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1004,8 +1137,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1114,4 +1247,214 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.85546875" customWidth="1"/>
+    <col min="3" max="3" width="23.5703125" customWidth="1"/>
+    <col min="4" max="4" width="29.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="H1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="150">
+      <c r="A2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="60">
+      <c r="B3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="60">
+      <c r="B4" t="s">
+        <v>103</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="135">
+      <c r="B5" t="s">
+        <v>104</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="90">
+      <c r="A7" t="s">
+        <v>105</v>
+      </c>
+      <c r="B7" t="s">
+        <v>106</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="45">
+      <c r="B8" t="s">
+        <v>107</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="75">
+      <c r="B9" t="s">
+        <v>108</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="90">
+      <c r="A10" t="s">
+        <v>109</v>
+      </c>
+      <c r="B10" t="s">
+        <v>110</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="135">
+      <c r="B11" t="s">
+        <v>111</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="90">
+      <c r="B12" t="s">
+        <v>89</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="75">
+      <c r="B13" t="s">
+        <v>112</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="135">
+      <c r="A14" t="s">
+        <v>113</v>
+      </c>
+      <c r="B14" t="s">
+        <v>114</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="150">
+      <c r="B15" t="s">
+        <v>115</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="195">
+      <c r="B16" t="s">
+        <v>116</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="60">
+      <c r="A17" t="s">
+        <v>117</v>
+      </c>
+      <c r="B17" t="s">
+        <v>118</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="75">
+      <c r="B18" t="s">
+        <v>119</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="90">
+      <c r="B19" t="s">
+        <v>120</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="150">
+      <c r="B20" t="s">
+        <v>121</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="210">
+      <c r="B21" t="s">
+        <v>138</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C19" r:id="rId1" display="https://www.netsuite.com/portal/resource/articles/inventory-management/freight.shtml"/>
+    <hyperlink ref="C20" r:id="rId2" display="https://www.netsuite.com/portal/resource/articles/inventory-management/inventory-carrying-costs.shtml"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added Aerospace KPI in Domain Excel
</commit_message>
<xml_diff>
--- a/Domains and KPI's.xlsx
+++ b/Domains and KPI's.xlsx
@@ -4,20 +4,21 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20055" windowHeight="7950" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="20055" windowHeight="7950" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="KPI Names" sheetId="1" r:id="rId1"/>
     <sheet name="Health Care Industry" sheetId="2" r:id="rId2"/>
     <sheet name="Automotive" sheetId="3" r:id="rId3"/>
     <sheet name="Supply Chain Logistics" sheetId="4" r:id="rId4"/>
+    <sheet name="Aerospace" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="163">
   <si>
     <t>Domain</t>
   </si>
@@ -443,6 +444,69 @@
   </si>
   <si>
     <t>Transportation costs are the group of metrics that track an order’s price from beginning to end. This metric includes order processing, administration, inventory carrying costs, warehousing and transportation costs</t>
+  </si>
+  <si>
+    <t>Satefy</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Building a safety culture in a plant should be intentional – from prevention to awareness to education to reporting. </t>
+  </si>
+  <si>
+    <t>First Yield Pass</t>
+  </si>
+  <si>
+    <t>First Pass Yield is the percentage of products that pass all quality inspections and tests without requiring rework or repairs.igh FPY rates indicate that products are built right the first time, reducing costs associated with rework and increasing customer satisfaction.</t>
+  </si>
+  <si>
+    <t>On Time Delivery</t>
+  </si>
+  <si>
+    <t>On-Time Delivery measures the percentage of products delivered to customers by the promised date.</t>
+  </si>
+  <si>
+    <t>Delivery</t>
+  </si>
+  <si>
+    <t>Cost Per Unit</t>
+  </si>
+  <si>
+    <t>Cost Per Unit tracks the total cost incurred to produce one unit of a product, including materials, labor, and overhead.</t>
+  </si>
+  <si>
+    <t>Manufacturing Lead Time</t>
+  </si>
+  <si>
+    <t>Manufacturing Lead Time measures the total time required to complete the production of a product, from the start of the manufacturing process to final delivery.</t>
+  </si>
+  <si>
+    <t>Supplier Quality Rating</t>
+  </si>
+  <si>
+    <t>Supplier Quality Rating assesses the performance and reliability of suppliers based on the quality of materials and components they provide.</t>
+  </si>
+  <si>
+    <t>ROI</t>
+  </si>
+  <si>
+    <t>Return on Investment measures the profitability of investments in equipment, technology, or projects by comparing the return to the investment cost.</t>
+  </si>
+  <si>
+    <t>Compliance Rate</t>
+  </si>
+  <si>
+    <t> Compliance Rate tracks the percentage of products and processes that adhere to industry regulations, standards, and contractual requirements.</t>
+  </si>
+  <si>
+    <t>Inventory Turn Over Rate</t>
+  </si>
+  <si>
+    <t>Inventory Turnover Ratio measures how often inventory is sold and replaced over a given period.</t>
+  </si>
+  <si>
+    <t>Scrap Rate</t>
+  </si>
+  <si>
+    <t>Scrap Rate measures the percentage of materials or products that are discarded due to defects or errors during the manufacturing process.</t>
   </si>
 </sst>
 </file>
@@ -1253,8 +1317,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1457,4 +1521,118 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="106.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B2" t="s">
+        <v>142</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="45">
+      <c r="B3" t="s">
+        <v>144</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="B4" t="s">
+        <v>146</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="30">
+      <c r="B5" t="s">
+        <v>149</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="30">
+      <c r="B6" t="s">
+        <v>151</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="30">
+      <c r="B7" t="s">
+        <v>153</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="30">
+      <c r="B8" t="s">
+        <v>155</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="30">
+      <c r="B9" t="s">
+        <v>157</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="B10" t="s">
+        <v>159</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="30">
+      <c r="B11" t="s">
+        <v>161</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>162</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added more KPI for Aviation Ground staff in Domain KPI.
</commit_message>
<xml_diff>
--- a/Domains and KPI's.xlsx
+++ b/Domains and KPI's.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="178">
   <si>
     <t>Domain</t>
   </si>
@@ -507,6 +507,51 @@
   </si>
   <si>
     <t>Scrap Rate measures the percentage of materials or products that are discarded due to defects or errors during the manufacturing process.</t>
+  </si>
+  <si>
+    <t>Ground Staff Maintenance</t>
+  </si>
+  <si>
+    <t>Turnaround Time per Aircraft Type</t>
+  </si>
+  <si>
+    <t>Total time elapsed between block-on and block-off. This metric must consider aircraft configuration, gate location, and local constraints.</t>
+  </si>
+  <si>
+    <t>Average Delay per Flight</t>
+  </si>
+  <si>
+    <t>Captures the mean delay duration across all flights. Used in conjunction with root-cause analysis, it helps isolate the share of delay attributable to ground handling.</t>
+  </si>
+  <si>
+    <t>Mishandled Baggage Index (MBI)</t>
+  </si>
+  <si>
+    <t>Measures the percentage of bags delivered to the correct flight or carousel within SLA thresholds.</t>
+  </si>
+  <si>
+    <t>Delays per 100 Flight Legs</t>
+  </si>
+  <si>
+    <t>Quantifies how frequently delays occur across a standardized number of flights, helping detect systemic issues in scheduling or execution.</t>
+  </si>
+  <si>
+    <t>Ground Incident Rate per 1,000 Flights</t>
+  </si>
+  <si>
+    <t>Tracks safety-related deviations, including equipment collisions, misconnects, and FOD events.</t>
+  </si>
+  <si>
+    <t>Staff Task Compliance</t>
+  </si>
+  <si>
+    <t>Monitors procedural adherence based on logged task completions, often integrated with mobile crew management systems.</t>
+  </si>
+  <si>
+    <t>Passenger Touchpoint SLA Compliance</t>
+  </si>
+  <si>
+    <t>(e.g., wheelchair delivery, cabin cleaning readiness) connects service-level commitments to operational execution.</t>
   </si>
 </sst>
 </file>
@@ -1525,15 +1570,16 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="106.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1631,6 +1677,65 @@
         <v>162</v>
       </c>
     </row>
+    <row r="13" spans="1:3" ht="30">
+      <c r="A13" t="s">
+        <v>163</v>
+      </c>
+      <c r="B13" t="s">
+        <v>164</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="30">
+      <c r="B14" t="s">
+        <v>166</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="B15" t="s">
+        <v>168</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="30">
+      <c r="B16" t="s">
+        <v>170</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3">
+      <c r="B17" t="s">
+        <v>172</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" ht="30">
+      <c r="B18" t="s">
+        <v>174</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3">
+      <c r="B19" t="s">
+        <v>176</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>177</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added more KPI for Avaition Domain KPI.
</commit_message>
<xml_diff>
--- a/Domains and KPI's.xlsx
+++ b/Domains and KPI's.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="200">
   <si>
     <t>Domain</t>
   </si>
@@ -552,6 +552,72 @@
   </si>
   <si>
     <t>(e.g., wheelchair delivery, cabin cleaning readiness) connects service-level commitments to operational execution.</t>
+  </si>
+  <si>
+    <t>Profits and Customer Satisfaction</t>
+  </si>
+  <si>
+    <t>Revenue per Kilometer</t>
+  </si>
+  <si>
+    <t>Volume of passanger carried by aircraft</t>
+  </si>
+  <si>
+    <t>Passanger Yield</t>
+  </si>
+  <si>
+    <t>Passenger yield measures the average revenue received per passenger kilometre flown, calculated by dividing total passenger revenue by the total number of revenue passenger kilometres (RPK).</t>
+  </si>
+  <si>
+    <t>Revenue Per Available Seat Kilometer</t>
+  </si>
+  <si>
+    <t>Revenue per Available Seat Kilometer (RASK) measures the airline’s revenue generated per kilometre for each seat available for sale. It’s calculated by dividing total passenger revenue by available seat kilometres (ASK).</t>
+  </si>
+  <si>
+    <t>Revenue per kilometer</t>
+  </si>
+  <si>
+    <t>. It indicates how effectively an airline monetises the distance passengers travel, reflecting pricing strategies and revenue generation efficiency.</t>
+  </si>
+  <si>
+    <t>Cost Per Available Seat Kilometer</t>
+  </si>
+  <si>
+    <t>Cost per Available Seat Kilometer (CASK) measures the operating expenses incurred by an airline for each available seat kilometer (ASK), calculated by dividing total operating expenses by ASK.</t>
+  </si>
+  <si>
+    <t>Break Even Loader</t>
+  </si>
+  <si>
+    <t>Break-even Load Factor (BLF) is the passenger load factor at which an airline covers all its costs with revenue, resulting in neither profit nor loss. It helps determine the minimum occupancy level required for flights to break even financially.</t>
+  </si>
+  <si>
+    <t>Operational KPI</t>
+  </si>
+  <si>
+    <t>On Time Performance</t>
+  </si>
+  <si>
+    <t>On-Time Performance (OTP) measures the percentage of flights that depart and arrive within a specified timeframe of their scheduled times,</t>
+  </si>
+  <si>
+    <t>Baggage Handling</t>
+  </si>
+  <si>
+    <t>Baggage Handling Performance measures the rate at which baggage is mishandled, encompassing lost, delayed, or damaged luggage incidents. It directly reflects the effectiveness of an airline’s baggage handling processes and operational efficiency.</t>
+  </si>
+  <si>
+    <t>Customer Satisfaction Index</t>
+  </si>
+  <si>
+    <t>Customer Satisfaction Index (CSI) is a metric that quantifies passengers’ satisfaction levels with various aspects of airline services, including check-in, onboard experience, and customer service interactions.</t>
+  </si>
+  <si>
+    <t>Net Promoter Score</t>
+  </si>
+  <si>
+    <t>Net Promoter Score (NPS) assesses customer loyalty and satisfaction based on the likelihood of passengers recommending the airline to others. It categorises customers as promoters (loyal enthusiasts), detractors (unhappy customers), or passives (neutral customers).</t>
   </si>
 </sst>
 </file>
@@ -1570,10 +1636,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22:C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1712,7 +1778,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="17" spans="2:3">
+    <row r="17" spans="1:3">
       <c r="B17" t="s">
         <v>172</v>
       </c>
@@ -1720,7 +1786,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="18" spans="2:3" ht="30">
+    <row r="18" spans="1:3" ht="30">
       <c r="B18" t="s">
         <v>174</v>
       </c>
@@ -1728,13 +1794,102 @@
         <v>175</v>
       </c>
     </row>
-    <row r="19" spans="2:3">
+    <row r="19" spans="1:3">
       <c r="B19" t="s">
         <v>176</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>177</v>
       </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" t="s">
+        <v>178</v>
+      </c>
+      <c r="B21" t="s">
+        <v>179</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="30">
+      <c r="B22" t="s">
+        <v>181</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="30">
+      <c r="B23" t="s">
+        <v>183</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="30">
+      <c r="B24" t="s">
+        <v>185</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="30">
+      <c r="B25" t="s">
+        <v>187</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="45">
+      <c r="B26" t="s">
+        <v>189</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="30">
+      <c r="A27" t="s">
+        <v>191</v>
+      </c>
+      <c r="B27" t="s">
+        <v>192</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="45">
+      <c r="B28" t="s">
+        <v>194</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="30">
+      <c r="B29" t="s">
+        <v>196</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="45">
+      <c r="B30" t="s">
+        <v>198</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="C31" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Started with adding KPI for insurance domain
</commit_message>
<xml_diff>
--- a/Domains and KPI's.xlsx
+++ b/Domains and KPI's.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20055" windowHeight="7950" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="20055" windowHeight="7950" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="KPI Names" sheetId="1" r:id="rId1"/>
@@ -12,13 +12,14 @@
     <sheet name="Automotive" sheetId="3" r:id="rId3"/>
     <sheet name="Supply Chain Logistics" sheetId="4" r:id="rId4"/>
     <sheet name="Aerospace" sheetId="5" r:id="rId5"/>
+    <sheet name="Insurance" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="224">
   <si>
     <t>Domain</t>
   </si>
@@ -618,6 +619,78 @@
   </si>
   <si>
     <t>Net Promoter Score (NPS) assesses customer loyalty and satisfaction based on the likelihood of passengers recommending the airline to others. It categorises customers as promoters (loyal enthusiasts), detractors (unhappy customers), or passives (neutral customers).</t>
+  </si>
+  <si>
+    <t>Sales</t>
+  </si>
+  <si>
+    <t>Quote Rate</t>
+  </si>
+  <si>
+    <t>The quote rate measures how many quotes a staff member has been able to provide compared to the number of leads they have contacted.</t>
+  </si>
+  <si>
+    <t>Quota Rate</t>
+  </si>
+  <si>
+    <t>The quota rate is used to measure the performance of staff in meeting their sales targets. </t>
+  </si>
+  <si>
+    <t>Contract Rate</t>
+  </si>
+  <si>
+    <t>This KPI measures how many leads a staff member was able to contact vs. the total number of leads they reached out to.</t>
+  </si>
+  <si>
+    <t>Leads</t>
+  </si>
+  <si>
+    <t>a person who has shown interest in a company's insurance products or services and is a potential customer</t>
+  </si>
+  <si>
+    <t>Number of Referrals</t>
+  </si>
+  <si>
+    <t> This insurance KPI measures how many new clients were referred by existing clients against the total number of new clients over a given time period.</t>
+  </si>
+  <si>
+    <t>Bind Rate</t>
+  </si>
+  <si>
+    <t>The bind rate insurance KPI is useful as it measures individual performance of staff, showing who has the skills to close a deal. The bind rate is the percentage of quotes that are converted into legally binding policies.</t>
+  </si>
+  <si>
+    <t>Percentage Pending</t>
+  </si>
+  <si>
+    <t>This measures how many policies at any given time are pending approval as a percentage of the total number of policies established.</t>
+  </si>
+  <si>
+    <t>Sales Growth Rate</t>
+  </si>
+  <si>
+    <t>This insurance performance metric measures how much a company’s sales have increased (or decreased) over a specific period.</t>
+  </si>
+  <si>
+    <t>New Policies per Agent</t>
+  </si>
+  <si>
+    <t>You want to know who your top performing agent is, don’t you? This insurance metric helps companies keep track of who their star performers are, as well as bringing about some healthy competition between agents.</t>
+  </si>
+  <si>
+    <t>Retention Rate</t>
+  </si>
+  <si>
+    <t>Obtaining new clients can be a costly and time-consuming process. In fact, it is much more profitable for companies if they can renew an exiting policy</t>
+  </si>
+  <si>
+    <t>Policies In-Force per Agent</t>
+  </si>
+  <si>
+    <t>his insurance metric isn’t targeted at the agent specific level. It takes the total number of policies in-force and divides it by the total number of agents on staff. This insurance KPI can be used in conjunction with the retention rate metric and the sales growth rate to try and identify where inefficiencies are occurring.</t>
+  </si>
+  <si>
+    <t>Reference Link : https://insightsoftware.com/blog/best-insurance-kpis-and-metrics/</t>
   </si>
 </sst>
 </file>
@@ -968,7 +1041,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -1638,7 +1711,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C22" sqref="C22:C31"/>
     </sheetView>
   </sheetViews>
@@ -1895,4 +1968,130 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="29.85546875" customWidth="1"/>
+    <col min="2" max="2" width="48" customWidth="1"/>
+    <col min="3" max="3" width="142.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>200</v>
+      </c>
+      <c r="B2" t="s">
+        <v>201</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="E2" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="B3" t="s">
+        <v>203</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="B4" t="s">
+        <v>205</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="B5" t="s">
+        <v>207</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="B6" t="s">
+        <v>209</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="30">
+      <c r="B7" t="s">
+        <v>211</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="B8" t="s">
+        <v>213</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="B9" t="s">
+        <v>215</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="30">
+      <c r="B10" t="s">
+        <v>217</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="B11" t="s">
+        <v>219</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="45">
+      <c r="B12" t="s">
+        <v>221</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>222</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added more KPI's for insurance sheet
</commit_message>
<xml_diff>
--- a/Domains and KPI's.xlsx
+++ b/Domains and KPI's.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="253">
   <si>
     <t>Domain</t>
   </si>
@@ -691,6 +691,93 @@
   </si>
   <si>
     <t>Reference Link : https://insightsoftware.com/blog/best-insurance-kpis-and-metrics/</t>
+  </si>
+  <si>
+    <t>Claims</t>
+  </si>
+  <si>
+    <t>Average Cost Per Claim </t>
+  </si>
+  <si>
+    <t>In the insurance industry, you are going to have to pay out on claims. That is just the nature of the business. The question is, how much are you going to be paying out? This insurance performance indicator helps estimate this by figuring out the average cost of each claim made</t>
+  </si>
+  <si>
+    <t>Claim Frequency</t>
+  </si>
+  <si>
+    <t> This key insurance metric measures the likelihood of a loss. It does this by predicting how many claims are to be expected based on the number of policies outstanding. This can help a company manage cashflows, risk exposure, and rate setting.</t>
+  </si>
+  <si>
+    <t>Components of Claim Costs (CCC) </t>
+  </si>
+  <si>
+    <t>The CCC metric seeks to provide insight into what costs are associated with a claim. The costs are generally associated with the following items: legal fees, time to settle, administration costs, and report delays. </t>
+  </si>
+  <si>
+    <t>Average Time to Settle a Claim</t>
+  </si>
+  <si>
+    <t>he claim settlement time should be used to monitor different policy types as more complicated policies will obviously take longer.</t>
+  </si>
+  <si>
+    <t>Client Satisfaction</t>
+  </si>
+  <si>
+    <t>Client satisfaction is probably best represented in client retention and policy renewal</t>
+  </si>
+  <si>
+    <t>Calls Handled within 24 Hours</t>
+  </si>
+  <si>
+    <t>This insurance metric is used to determine how efficient and effective a company’s claims resolution team is. This KPI shouldn’t be used entirely by itself. A company should also consider how many calls the team receives.</t>
+  </si>
+  <si>
+    <t>Underwriting Cycle Time</t>
+  </si>
+  <si>
+    <t> This insurance performance indicator measures the number of days it takes the underwriting department of a company to process an insurance policy application. This top insurance KPI can highlight inefficient underwriters, which can have a negative impact on client satisfaction. </t>
+  </si>
+  <si>
+    <t>Claims Ratio </t>
+  </si>
+  <si>
+    <t>The claims ratio is a very powerful insurance metric. It takes the number of claims made and divides them by the amount of insurance premium earned for a specific period.</t>
+  </si>
+  <si>
+    <t>Financial</t>
+  </si>
+  <si>
+    <t>Expense Ratio</t>
+  </si>
+  <si>
+    <t>The expense ratio performance metric compares the company’s total expenses to the premiums it generates over a specific time period. </t>
+  </si>
+  <si>
+    <t>Loss Ratio</t>
+  </si>
+  <si>
+    <t>his insurance KPI divides the total claims payout and divides it by the total premium revenue. A high loss ratio may indicate that policy premiums are set too low.</t>
+  </si>
+  <si>
+    <t>Average Revenue Per Client</t>
+  </si>
+  <si>
+    <t>We can use this insurance metric to determine the maximum amount of money a company is willing to spend to obtain a new client</t>
+  </si>
+  <si>
+    <t>Cost Per Quote</t>
+  </si>
+  <si>
+    <t>The cost per quote takes into consideration all the costs that the company incurs in order to get a quote in front of a potential client.</t>
+  </si>
+  <si>
+    <t>Cost Per Bind</t>
+  </si>
+  <si>
+    <t>The cost per bind metric determines the incremental cost of binding a new policy. It essentially represents the price a company pays to obtain a new client.</t>
+  </si>
+  <si>
+    <t>This is the official measure of “are you profitable.” If your net income isn’t positive, you aren’t making a profit. But, when you do have a net income that is positive, just divide it by the total revenue.</t>
   </si>
 </sst>
 </file>
@@ -1972,10 +2059,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2090,6 +2177,127 @@
         <v>222</v>
       </c>
     </row>
+    <row r="13" spans="1:5" ht="30">
+      <c r="A13" t="s">
+        <v>224</v>
+      </c>
+      <c r="B13" t="s">
+        <v>225</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="30">
+      <c r="B14" t="s">
+        <v>227</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="30">
+      <c r="B15" t="s">
+        <v>229</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="B16" t="s">
+        <v>231</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="B17" t="s">
+        <v>233</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="30">
+      <c r="B18" t="s">
+        <v>235</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="30">
+      <c r="B19" t="s">
+        <v>237</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="30">
+      <c r="B20" t="s">
+        <v>239</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="C21" s="2"/>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" t="s">
+        <v>241</v>
+      </c>
+      <c r="B22" t="s">
+        <v>242</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="30">
+      <c r="B23" t="s">
+        <v>244</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="B24" t="s">
+        <v>246</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="B25" t="s">
+        <v>248</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="B26" t="s">
+        <v>250</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="30">
+      <c r="B27" t="s">
+        <v>70</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>252</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>